<commit_message>
mais testes e correção no codigo
</commit_message>
<xml_diff>
--- a/documentacao/testes_planilha.xlsx
+++ b/documentacao/testes_planilha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princesa\Documents\Bandtec\GIT-Bandtec\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED9F585-CE57-4C08-9AE8-328BD9F51A74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53492463-A5C7-4FC9-BD20-ED028D260409}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C247229E-688C-4DEF-8E53-CD8B5F4C2F4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C247229E-688C-4DEF-8E53-CD8B5F4C2F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Testes Unitários" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Testes Unitários</t>
   </si>
@@ -82,13 +82,37 @@
   </si>
   <si>
     <t>Ao "Alterar a senha" deve ser enviado um e-mail para a adm solicitando uma senha nova</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Tentar mudar de pagina</t>
+  </si>
+  <si>
+    <t>ao clicar em algum link, mudar para a pagina esperada</t>
+  </si>
+  <si>
+    <t>site privado</t>
+  </si>
+  <si>
+    <t>testar botões do menu</t>
+  </si>
+  <si>
+    <t>ao clicar nos botões, ir para a parte correspondente da pagina</t>
+  </si>
+  <si>
+    <t>testar os simuladores financeiros</t>
+  </si>
+  <si>
+    <t>ao clicar em "simular", em cada uma das opções, deve ser exibido um alert com o resultado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +131,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -141,12 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +497,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,28 +510,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -558,25 +591,53 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -638,6 +699,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizando Planilha de testes e requisitos
</commit_message>
<xml_diff>
--- a/documentacao/testes_planilha.xlsx
+++ b/documentacao/testes_planilha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princesa\Documents\Bandtec\GIT-Bandtec\grupo9-ads\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53492463-A5C7-4FC9-BD20-ED028D260409}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27271B35-4FAD-47A7-8C89-2B6BAEAA4436}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C247229E-688C-4DEF-8E53-CD8B5F4C2F4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C247229E-688C-4DEF-8E53-CD8B5F4C2F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Testes Unitários" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Testes Unitários</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Ao "Alterar a senha" deve ser enviado um e-mail para a adm solicitando uma senha nova</t>
   </si>
   <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>Tentar mudar de pagina</t>
   </si>
   <si>
@@ -106,6 +103,30 @@
   </si>
   <si>
     <t>ao clicar em "simular", em cada uma das opções, deve ser exibido um alert com o resultado</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Site privado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testar os botões de sair </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao clicar nos botões de sair em todas as abas, o usuário deverá ser redirecionado para o site institucional </t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado obtido foi o mesmo que o esperado </t>
+  </si>
+  <si>
+    <t>Bater modelo conceitual com dados requeridos no cadastro</t>
+  </si>
+  <si>
+    <t>Que todos os dados requeridos sejam iguais</t>
   </si>
 </sst>
 </file>
@@ -165,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -176,10 +197,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D646B23-A933-410D-9BF0-D1D68AA0FB5F}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,19 +533,19 @@
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="46.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="5" max="5" width="36" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -535,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -563,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -577,7 +604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -591,80 +618,113 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>